<commit_message>
Added mislabel report files
</commit_message>
<xml_diff>
--- a/src/models/RF_vs_GNB_mislabel_comparison.xlsx
+++ b/src/models/RF_vs_GNB_mislabel_comparison.xlsx
@@ -32,9 +32,6 @@
     <t>Actual Collection</t>
   </si>
   <si>
-    <t>RF Predictetion</t>
-  </si>
-  <si>
     <t>GNB Prediction</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>web-wikipedia2009</t>
   </si>
   <si>
-    <t>socfb-A-anon</t>
-  </si>
-  <si>
     <t>socfb-OR</t>
   </si>
   <si>
@@ -174,6 +168,12 @@
   </si>
   <si>
     <t>bn-mouse-visual-cortex-2</t>
+  </si>
+  <si>
+    <t>RF Prediction</t>
+  </si>
+  <si>
+    <t>socfb-B-anon</t>
   </si>
 </sst>
 </file>
@@ -500,12 +500,12 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
@@ -522,39 +522,39 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1">
         <v>0.99999774794095797</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="2">
         <v>2.21874008835468E-6</v>
@@ -562,22 +562,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1">
         <v>0.957938130707507</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" s="2">
         <v>4.1953226995189101E-2</v>
@@ -585,22 +585,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1">
         <v>0.99909209906097196</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" s="2">
         <v>9.0790088299325502E-4</v>
@@ -608,22 +608,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
@@ -631,22 +631,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1">
         <v>0.62326503926820198</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" s="2">
         <v>0.376410052628111</v>
@@ -654,22 +654,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1">
         <v>0.99534696600414596</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" s="2">
         <v>4.0334017559115901E-3</v>
@@ -677,22 +677,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1">
         <v>0.99999883270168199</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" s="2">
         <v>1.16729831673034E-6</v>
@@ -700,22 +700,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1">
         <v>0.970526960465116</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G9" s="2">
         <v>2.9466989914096901E-2</v>
@@ -723,22 +723,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1">
         <v>0.96912480029880599</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G10" s="2">
         <v>2.8897239266194901E-2</v>
@@ -746,22 +746,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="1">
         <v>0.94901556720256897</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G11" s="2">
         <v>5.0141303058365699E-2</v>
@@ -769,22 +769,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G12" s="2">
         <v>1.47522468043317E-117</v>
@@ -792,22 +792,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1">
         <v>0.95587079682613296</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="2">
         <v>2.5903691341316201E-2</v>
@@ -815,22 +815,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" s="1">
         <v>0.99727665956002898</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G14" s="2">
         <v>2.6655417933655898E-3</v>
@@ -838,22 +838,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" s="1">
         <v>0.64166143555615396</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15" s="2">
         <v>0.35687191319512401</v>
@@ -861,22 +861,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E16" s="1">
-        <v>0.62112558497081005</v>
+        <v>0.71809776051547003</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G16" s="2">
         <v>0.37855867805294202</v>
@@ -884,22 +884,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="1">
         <v>0.99343077708212502</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G17" s="2">
         <v>6.4247310350073498E-3</v>
@@ -907,22 +907,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" s="1">
         <v>0.99999999485135005</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G18" s="2">
         <v>5.1074418873000397E-9</v>
@@ -930,22 +930,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19" s="1">
         <v>0.99780514683761201</v>
       </c>
       <c r="F19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G19" s="2">
         <v>2.1945590162829802E-3</v>
@@ -953,22 +953,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20" s="1">
         <v>0.67955903940516904</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G20" s="2">
         <v>0.30947814815506097</v>
@@ -976,22 +976,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E21" s="1">
         <v>0.99999871425769105</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G21" s="2">
         <v>1.25889424659043E-6</v>
@@ -999,22 +999,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22" s="1">
         <v>0.96937544631182404</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G22" s="2">
         <v>2.9367712095381401E-2</v>
@@ -1022,22 +1022,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E23" s="1">
         <v>0.56210324370070197</v>
       </c>
       <c r="F23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G23" s="2">
         <v>0.43632492932259898</v>
@@ -1045,22 +1045,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E24" s="1">
         <v>0.99682114005481204</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G24" s="2">
         <v>3.1788599410723698E-3</v>
@@ -1068,22 +1068,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25" s="1">
         <v>0.97389499540368196</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G25" s="2">
         <v>2.5170296874572701E-2</v>
@@ -1091,22 +1091,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E26" s="1">
         <v>0.97731255171503395</v>
       </c>
       <c r="F26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G26" s="2">
         <v>2.2530181903861898E-2</v>
@@ -1114,22 +1114,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E27" s="1">
         <v>0.99999293838093795</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G27" s="2">
         <v>6.91574006010394E-6</v>
@@ -1137,22 +1137,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E28" s="1">
         <v>0.98598988892280004</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G28" s="2">
         <v>1.4005843789366E-2</v>
@@ -1160,22 +1160,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E29" s="1">
         <v>0.98247674162142096</v>
       </c>
       <c r="F29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G29" s="2">
         <v>1.7521060466619401E-2</v>
@@ -1183,22 +1183,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E30" s="1">
         <v>0.99999583510263501</v>
       </c>
       <c r="F30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G30" s="2">
         <v>3.4416913455482199E-6</v>
@@ -1206,22 +1206,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G31" s="2">
         <v>1.11721704668002E-32</v>
@@ -1229,22 +1229,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G32" s="2">
         <v>4.7759123124647697E-22</v>
@@ -1252,22 +1252,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E33" s="1">
         <v>0.99999943100188005</v>
       </c>
       <c r="F33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G33" s="2">
         <v>5.6419603875406702E-7</v>
@@ -1275,22 +1275,22 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E34" s="1">
         <v>0.99999461425724001</v>
       </c>
       <c r="F34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G34" s="2">
         <v>5.3857414302611001E-6</v>

</xml_diff>

<commit_message>
tested misc networks with comb collections
</commit_message>
<xml_diff>
--- a/src/models/RF_vs_GNB_mislabel_comparison.xlsx
+++ b/src/models/RF_vs_GNB_mislabel_comparison.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="50">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="47">
   <si>
     <t>Actual Collection</t>
   </si>
@@ -35,15 +32,9 @@
     <t>GNB Prediction</t>
   </si>
   <si>
-    <t>Prediction Probability</t>
-  </si>
-  <si>
     <t>2nd Prediction</t>
   </si>
   <si>
-    <t>2nd Highest Probability</t>
-  </si>
-  <si>
     <t>web-EPA</t>
   </si>
   <si>
@@ -92,18 +83,12 @@
     <t>web-spam</t>
   </si>
   <si>
-    <t>Social/Facebook) Networks</t>
-  </si>
-  <si>
     <t>web-uk-2005</t>
   </si>
   <si>
     <t>web-webbase-2001</t>
   </si>
   <si>
-    <t>Social/Retweet Networks</t>
-  </si>
-  <si>
     <t>web-wiki-ch-internal</t>
   </si>
   <si>
@@ -125,9 +110,6 @@
     <t>soc-douban</t>
   </si>
   <si>
-    <t>Retweet/Web Networks</t>
-  </si>
-  <si>
     <t>soc-gplus</t>
   </si>
   <si>
@@ -164,9 +146,6 @@
     <t>bn-mouse-visual-cortex-1</t>
   </si>
   <si>
-    <t>Cheminformatics Networks</t>
-  </si>
-  <si>
     <t>bn-mouse-visual-cortex-2</t>
   </si>
   <si>
@@ -174,6 +153,18 @@
   </si>
   <si>
     <t>socfb-B-anon</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Probability</t>
+  </si>
+  <si>
+    <t>2nd Probability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheminformatics </t>
   </si>
 </sst>
 </file>
@@ -221,7 +212,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -232,6 +230,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Random_Forest_Milabel" displayName="Random_Forest_Milabel" ref="A1:G34" totalsRowShown="0">
+  <autoFilter ref="A1:G34"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Graph"/>
+    <tableColumn id="2" name="Actual Collection"/>
+    <tableColumn id="3" name="RF Prediction"/>
+    <tableColumn id="4" name="GNB Prediction"/>
+    <tableColumn id="5" name=" Probability" dataDxfId="1"/>
+    <tableColumn id="6" name="2nd Prediction"/>
+    <tableColumn id="7" name="2nd Probability" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -500,61 +514,61 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1">
         <v>0.99999774794095797</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G2" s="2">
         <v>2.21874008835468E-6</v>
@@ -562,22 +576,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1">
         <v>0.957938130707507</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G3" s="2">
         <v>4.1953226995189101E-2</v>
@@ -585,22 +599,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1">
         <v>0.99909209906097196</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G4" s="2">
         <v>9.0790088299325502E-4</v>
@@ -608,22 +622,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
@@ -631,22 +645,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1">
         <v>0.62326503926820198</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G6" s="2">
         <v>0.376410052628111</v>
@@ -654,22 +668,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E7" s="1">
         <v>0.99534696600414596</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G7" s="2">
         <v>4.0334017559115901E-3</v>
@@ -677,22 +691,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E8" s="1">
         <v>0.99999883270168199</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2">
         <v>1.16729831673034E-6</v>
@@ -700,22 +714,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E9" s="1">
         <v>0.970526960465116</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G9" s="2">
         <v>2.9466989914096901E-2</v>
@@ -723,22 +737,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E10" s="1">
         <v>0.96912480029880599</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G10" s="2">
         <v>2.8897239266194901E-2</v>
@@ -746,22 +760,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E11" s="1">
         <v>0.94901556720256897</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G11" s="2">
         <v>5.0141303058365699E-2</v>
@@ -769,22 +783,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G12" s="2">
         <v>1.47522468043317E-117</v>
@@ -792,22 +806,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E13" s="1">
         <v>0.95587079682613296</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G13" s="2">
         <v>2.5903691341316201E-2</v>
@@ -815,22 +829,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E14" s="1">
         <v>0.99727665956002898</v>
       </c>
       <c r="F14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G14" s="2">
         <v>2.6655417933655898E-3</v>
@@ -838,22 +852,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E15" s="1">
         <v>0.64166143555615396</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G15" s="2">
         <v>0.35687191319512401</v>
@@ -861,22 +875,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E16" s="1">
         <v>0.71809776051547003</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G16" s="2">
         <v>0.37855867805294202</v>
@@ -884,22 +898,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E17" s="1">
         <v>0.99343077708212502</v>
       </c>
       <c r="F17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G17" s="2">
         <v>6.4247310350073498E-3</v>
@@ -907,22 +921,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E18" s="1">
         <v>0.99999999485135005</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G18" s="2">
         <v>5.1074418873000397E-9</v>
@@ -930,22 +944,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E19" s="1">
         <v>0.99780514683761201</v>
       </c>
       <c r="F19" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G19" s="2">
         <v>2.1945590162829802E-3</v>
@@ -953,22 +967,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E20" s="1">
         <v>0.67955903940516904</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G20" s="2">
         <v>0.30947814815506097</v>
@@ -976,22 +990,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1">
         <v>0.99999871425769105</v>
       </c>
       <c r="F21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G21" s="2">
         <v>1.25889424659043E-6</v>
@@ -999,22 +1013,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E22" s="1">
         <v>0.96937544631182404</v>
       </c>
       <c r="F22" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G22" s="2">
         <v>2.9367712095381401E-2</v>
@@ -1022,22 +1036,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E23" s="1">
         <v>0.56210324370070197</v>
       </c>
       <c r="F23" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G23" s="2">
         <v>0.43632492932259898</v>
@@ -1045,22 +1059,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E24" s="1">
         <v>0.99682114005481204</v>
       </c>
       <c r="F24" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G24" s="2">
         <v>3.1788599410723698E-3</v>
@@ -1068,22 +1082,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E25" s="1">
         <v>0.97389499540368196</v>
       </c>
       <c r="F25" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G25" s="2">
         <v>2.5170296874572701E-2</v>
@@ -1091,22 +1105,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E26" s="1">
         <v>0.97731255171503395</v>
       </c>
       <c r="F26" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G26" s="2">
         <v>2.2530181903861898E-2</v>
@@ -1114,22 +1128,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E27" s="1">
         <v>0.99999293838093795</v>
       </c>
       <c r="F27" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G27" s="2">
         <v>6.91574006010394E-6</v>
@@ -1137,22 +1151,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E28" s="1">
         <v>0.98598988892280004</v>
       </c>
       <c r="F28" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G28" s="2">
         <v>1.4005843789366E-2</v>
@@ -1160,22 +1174,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E29" s="1">
         <v>0.98247674162142096</v>
       </c>
       <c r="F29" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G29" s="2">
         <v>1.7521060466619401E-2</v>
@@ -1183,22 +1197,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E30" s="1">
         <v>0.99999583510263501</v>
       </c>
       <c r="F30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G30" s="2">
         <v>3.4416913455482199E-6</v>
@@ -1206,22 +1220,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G31" s="2">
         <v>1.11721704668002E-32</v>
@@ -1229,22 +1243,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G32" s="2">
         <v>4.7759123124647697E-22</v>
@@ -1252,22 +1266,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
         <v>46</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E33" s="1">
         <v>0.99999943100188005</v>
       </c>
       <c r="F33" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G33" s="2">
         <v>5.6419603875406702E-7</v>
@@ -1275,28 +1289,32 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E34" s="1">
         <v>0.99999461425724001</v>
       </c>
       <c r="F34" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G34" s="2">
         <v>5.3857414302611001E-6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>